<commit_message>
first version of evaluation
</commit_message>
<xml_diff>
--- a/other documents/evaluation/experiment-data.xlsx
+++ b/other documents/evaluation/experiment-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonv\Documents\Uni\Master\Master-Thesis\master-thesis\other documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonv\Documents\Uni\Master\Master-Thesis\master-thesis\other documents\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA8FFC0-F6AD-45F8-8C68-30137F58CC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7308087-CC1C-4348-A695-2608A66BDAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{74E725B0-5B7F-4207-B493-632C2DD28F84}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>job</t>
   </si>
@@ -270,6 +270,27 @@
   </si>
   <si>
     <t>overview of the devices I have is nice</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>non-technical</t>
+  </si>
+  <si>
+    <t>technical</t>
+  </si>
+  <si>
+    <t>age-group</t>
+  </si>
+  <si>
+    <t>&lt;30</t>
+  </si>
+  <si>
+    <t>&lt;40</t>
+  </si>
+  <si>
+    <t>&gt;=40</t>
   </si>
 </sst>
 </file>
@@ -626,15 +647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC7524D-5D90-4BFF-9A25-A0B83F25E75B}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +668,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -661,8 +688,14 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -675,8 +708,14 @@
       <c r="D3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -689,8 +728,14 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -703,8 +748,14 @@
       <c r="D5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -717,8 +768,14 @@
       <c r="D6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -731,8 +788,14 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -745,8 +808,14 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -759,8 +828,14 @@
       <c r="D9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -773,8 +848,14 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -786,6 +867,12 @@
       </c>
       <c r="D11">
         <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -795,10 +882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB2C15A-A61B-4C41-9070-8D5A88F296C0}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +893,7 @@
     <col min="19" max="19" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -861,12 +948,8 @@
       <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="T1">
-        <f>AVERAGE(A:A)</f>
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20</v>
       </c>
@@ -921,12 +1004,8 @@
       <c r="R2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <f>AVERAGE(D:D)</f>
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -981,12 +1060,8 @@
       <c r="R3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <f>AVERAGE(G:G)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -1041,12 +1116,8 @@
       <c r="R4" s="1">
         <v>0</v>
       </c>
-      <c r="T4">
-        <f>AVERAGE(J:J)</f>
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -1101,12 +1172,8 @@
       <c r="R5" s="1">
         <v>1</v>
       </c>
-      <c r="T5">
-        <f>AVERAGE(M:M)</f>
-        <v>45.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -1161,12 +1228,8 @@
       <c r="R6">
         <v>1</v>
       </c>
-      <c r="T6">
-        <f>AVERAGE(P:P)</f>
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -1222,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1278,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>23</v>
       </c>
@@ -1334,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -1390,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
@@ -1454,15 +1517,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789C94B5-0D57-4747-B312-C62FB78DFB79}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H1" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1481,12 +1544,8 @@
       <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="H1">
-        <f>AVERAGE(A:A)</f>
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1505,12 +1564,8 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="H2">
-        <f>AVERAGE(B:B)</f>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1529,12 +1584,8 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="H3">
-        <f>AVERAGE(C:C)</f>
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -1553,12 +1604,8 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="H4">
-        <f>AVERAGE(D:D)</f>
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1577,12 +1624,8 @@
       <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="H5">
-        <f>AVERAGE(E:E)</f>
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1601,12 +1644,8 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="H6">
-        <f>AVERAGE(F:F)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1626,7 +1665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1646,7 +1685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1666,7 +1705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1686,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>

</xml_diff>